<commit_message>
Finer memory layout and prototype MMU
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -66,6 +67,39 @@
   </si>
   <si>
     <t>Loaded Program (overwrites ROM)</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Start Address</t>
+  </si>
+  <si>
+    <t>End Address</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>ROM/Later Program</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>GPU Registers/Objects</t>
+  </si>
+  <si>
+    <t>IO Registers</t>
+  </si>
+  <si>
+    <t>Audio Registers</t>
+  </si>
+  <si>
+    <t>Graphics and Shared</t>
   </si>
 </sst>
 </file>
@@ -437,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9178CA0-74B4-43BE-B552-DA32908998EC}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -488,22 +522,22 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -605,7 +639,7 @@
         <v>32768</v>
       </c>
       <c r="B9" s="1" t="str">
-        <f t="shared" ref="B7:B16" si="4">DEC2HEX(A9)</f>
+        <f t="shared" ref="B9:B16" si="4">DEC2HEX(A9)</f>
         <v>8000</v>
       </c>
       <c r="C9" s="1">
@@ -953,4 +987,411 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A333F48A-4545-44AF-8465-714E7B30E76A}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"$" &amp; DEC2HEX(A3, 4)</f>
+        <v>$0000</v>
+      </c>
+      <c r="C3">
+        <f>A3+4096-1</f>
+        <v>4095</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"$" &amp; DEC2HEX(C3, 4)</f>
+        <v>$0FFF</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+4096</f>
+        <v>4096</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B67" si="0">"$" &amp; DEC2HEX(A4, 4)</f>
+        <v>$1000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C18" si="1">A4+4096-1</f>
+        <v>8191</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D18" si="2">"$" &amp; DEC2HEX(C4, 4)</f>
+        <v>$1FFF</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A35" si="3">A4+4096</f>
+        <v>8192</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>$2000</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>12287</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>$2FFF</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="3"/>
+        <v>12288</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>$3000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>16383</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>$3FFF</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="3"/>
+        <v>16384</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>$4000</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>20479</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>$4FFF</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>20480</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>$5000</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>24575</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>$5FFF</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>24576</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>$6000</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>28671</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>$6FFF</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>28672</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>$7000</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>32767</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>$7FFF</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>$8000</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>36863</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>$8FFF</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>36864</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>$9000</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>40959</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>$9FFF</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>40960</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>$A000</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>45055</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>$AFFF</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>45056</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>$B000</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>49151</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>$BFFF</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>49152</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>$C000</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>53247</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>$CFFF</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>53248</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>$D000</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>57343</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>$DFFF</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>57344</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>$E000</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>61439</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>$EFFF</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>61440</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>$F000</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>65535</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>$FFFF</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic bootloader from stream. Gpu faulty.
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Addresses" sheetId="2" r:id="rId1"/>
-    <sheet name="Graphics" sheetId="3" r:id="rId2"/>
-    <sheet name="Tiles" sheetId="4" r:id="rId3"/>
+    <sheet name="AddressesIdea2" sheetId="7" r:id="rId2"/>
+    <sheet name="Uses" sheetId="6" r:id="rId3"/>
+    <sheet name="Graphics" sheetId="3" r:id="rId4"/>
+    <sheet name="Tiles" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -134,14 +136,112 @@
   </si>
   <si>
     <t>TileLen</t>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>MMUReg</t>
+  </si>
+  <si>
+    <t>Rand</t>
+  </si>
+  <si>
+    <t>MMUBank</t>
+  </si>
+  <si>
+    <t>GfxPlanes</t>
+  </si>
+  <si>
+    <t>Colours</t>
+  </si>
+  <si>
+    <t>Scanline</t>
+  </si>
+  <si>
+    <t>PlaneTypes</t>
+  </si>
+  <si>
+    <t>framenum</t>
+  </si>
+  <si>
+    <t>scanline</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>counters</t>
+  </si>
+  <si>
+    <t>GFXReg</t>
+  </si>
+  <si>
+    <t>GFXTiles</t>
+  </si>
+  <si>
+    <t>FPYRegs</t>
+  </si>
+  <si>
+    <t>GraphicsMem</t>
+  </si>
+  <si>
+    <t>InterruptTable</t>
+  </si>
+  <si>
+    <t>Len</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Mapped Registers</t>
+  </si>
+  <si>
+    <t>Bootloader puts program here</t>
+  </si>
+  <si>
+    <t>Graphics/Shared</t>
+  </si>
+  <si>
+    <t>Temp/Shared Variables</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>KB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,8 +269,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A333F48A-4545-44AF-8465-714E7B30E76A}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I18" sqref="A1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +608,7 @@
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -512,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -526,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -545,8 +655,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+4096</f>
         <v>4096</v>
@@ -566,8 +679,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A18" si="3">A4+4096</f>
         <v>8192</v>
@@ -587,8 +703,11 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>12288</v>
@@ -608,8 +727,11 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>16384</v>
@@ -629,8 +751,11 @@
       <c r="F7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>20480</v>
@@ -650,8 +775,11 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>24576</v>
@@ -671,8 +799,11 @@
       <c r="F9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>28672</v>
@@ -692,8 +823,11 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>32768</v>
@@ -716,8 +850,11 @@
       <c r="F11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>36864</v>
@@ -740,8 +877,11 @@
       <c r="F12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>40960</v>
@@ -764,8 +904,11 @@
       <c r="F13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>45056</v>
@@ -788,8 +931,11 @@
       <c r="F14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>49152</v>
@@ -812,8 +958,11 @@
       <c r="F15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>53248</v>
@@ -835,6 +984,9 @@
       </c>
       <c r="F16" t="s">
         <v>12</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -891,6 +1043,883 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C2689D-9543-405F-B6B3-E28019047877}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"$" &amp; DEC2HEX(A3, 4)</f>
+        <v>$0000</v>
+      </c>
+      <c r="C3">
+        <v>512</v>
+      </c>
+      <c r="D3" t="str">
+        <f>DEC2HEX(C3)</f>
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <f>A3+C3-1</f>
+        <v>511</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"$" &amp; DEC2HEX(E3, 4)</f>
+        <v>$01FF</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3">
+        <f>E3-A3+1</f>
+        <v>512</v>
+      </c>
+      <c r="K3" s="3">
+        <f>J3/1024</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>E3+1</f>
+        <v>512</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B19" si="0">"$" &amp; DEC2HEX(A4, 4)</f>
+        <v>$0200</v>
+      </c>
+      <c r="C4">
+        <f>4096-C3</f>
+        <v>3584</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D19" si="1">DEC2HEX(C4)</f>
+        <v>E00</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E19" si="2">A4+C4-1</f>
+        <v>4095</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F19" si="3">"$" &amp; DEC2HEX(E4, 4)</f>
+        <v>$0FFF</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="3">
+        <f>E4-A4+1</f>
+        <v>3584</v>
+      </c>
+      <c r="K4" s="3">
+        <f>J4/1024</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A19" si="4">E4+1</f>
+        <v>4096</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>$1000</v>
+      </c>
+      <c r="C5">
+        <v>4096</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>8191</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>$1FFF</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="4"/>
+        <v>8192</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>$2000</v>
+      </c>
+      <c r="C6">
+        <v>4096</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>12287</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v>$2FFF</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="4"/>
+        <v>12288</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>$3000</v>
+      </c>
+      <c r="C7">
+        <v>4096</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>16383</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>$3FFF</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="4"/>
+        <v>16384</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>$4000</v>
+      </c>
+      <c r="C8">
+        <v>4096</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>20479</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>$4FFF</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="4"/>
+        <v>20480</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>$5000</v>
+      </c>
+      <c r="C9">
+        <v>4096</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>24575</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>$5FFF</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="4"/>
+        <v>24576</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>$6000</v>
+      </c>
+      <c r="C10">
+        <v>4096</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>28671</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>$6FFF</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="4"/>
+        <v>28672</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>$7000</v>
+      </c>
+      <c r="C11">
+        <v>4096</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>32767</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>$7FFF</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="3">
+        <f>E11-A5+1</f>
+        <v>28672</v>
+      </c>
+      <c r="K11" s="3">
+        <f>J11/1024</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="4"/>
+        <v>32768</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>$8000</v>
+      </c>
+      <c r="C12">
+        <v>4096</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>36863</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>$8FFF</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="4"/>
+        <v>36864</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>$9000</v>
+      </c>
+      <c r="C13">
+        <v>4096</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>40959</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>$9FFF</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="4"/>
+        <v>40960</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>$A000</v>
+      </c>
+      <c r="C14">
+        <v>4096</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>45055</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>$AFFF</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="4"/>
+        <v>45056</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>$B000</v>
+      </c>
+      <c r="C15">
+        <v>4096</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>49151</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>$BFFF</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="4"/>
+        <v>49152</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>$C000</v>
+      </c>
+      <c r="C16">
+        <v>4096</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>53247</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>$CFFF</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="4"/>
+        <v>53248</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>$D000</v>
+      </c>
+      <c r="C17">
+        <v>4096</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>57343</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>$DFFF</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="4"/>
+        <v>57344</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>$E000</v>
+      </c>
+      <c r="C18">
+        <v>4096</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>61439</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>$EFFF</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="4"/>
+        <v>61440</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>$F000</v>
+      </c>
+      <c r="C19">
+        <v>4096</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>65535</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>$FFFF</v>
+      </c>
+      <c r="G19" s="2">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="3">
+        <f>E19-A12+1</f>
+        <v>32768</v>
+      </c>
+      <c r="K19" s="3">
+        <f>J19/1024</f>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC884A42-D2D6-402E-9371-0695EFE869F6}">
+  <dimension ref="D3:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>SUM(E4:E26)</f>
+        <v>323</v>
+      </c>
+      <c r="J3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E008FE-648B-4453-993C-DE8B315E1618}">
   <dimension ref="B2:J15"/>
   <sheetViews>
@@ -1074,11 +2103,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500CC495-F4F1-48E7-99EC-BC616FBB078F}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Word support for some opcodes. Bugfix with MMU.
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>KB</t>
+  </si>
+  <si>
+    <t>Screen Size</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C2689D-9543-405F-B6B3-E28019047877}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1065,7 @@
     <col min="11" max="11" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>E3+1</f>
         <v>512</v>
@@ -1195,7 +1198,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A19" si="4">E4+1</f>
         <v>4096</v>
@@ -1231,7 +1234,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="4"/>
         <v>8192</v>
@@ -1267,7 +1270,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="4"/>
         <v>12288</v>
@@ -1303,7 +1306,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="4"/>
         <v>16384</v>
@@ -1339,7 +1342,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="4"/>
         <v>20480</v>
@@ -1375,7 +1378,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="4"/>
         <v>24576</v>
@@ -1411,7 +1414,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="4"/>
         <v>28672</v>
@@ -1452,8 +1455,15 @@
         <f>J11/1024</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f>(320*256)/8</f>
+        <v>10240</v>
+      </c>
+      <c r="N11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="4"/>
         <v>32768</v>
@@ -1488,8 +1498,19 @@
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="str">
+        <f>DEC2HEX(M12)</f>
+        <v>8000</v>
+      </c>
+      <c r="M12">
+        <f>$A$12+($M$11*N12)</f>
+        <v>32768</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="4"/>
         <v>36864</v>
@@ -1524,8 +1545,19 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="str">
+        <f t="shared" ref="L13:L15" si="5">DEC2HEX(M13)</f>
+        <v>A800</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13:M15" si="6">$A$12+($M$11*N13)</f>
+        <v>43008</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="4"/>
         <v>40960</v>
@@ -1560,8 +1592,19 @@
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>D000</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="6"/>
+        <v>53248</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="4"/>
         <v>45056</v>
@@ -1596,8 +1639,19 @@
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>F800</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="6"/>
+        <v>63488</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="4"/>
         <v>49152</v>

</xml_diff>

<commit_message>
Virtual Memory Tests, and meshes/textures from stream
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Addresses" sheetId="2" r:id="rId1"/>
@@ -17,8 +17,10 @@
     <sheet name="Uses" sheetId="6" r:id="rId3"/>
     <sheet name="Graphics" sheetId="3" r:id="rId4"/>
     <sheet name="Tiles" sheetId="4" r:id="rId5"/>
+    <sheet name="Software MMU Calculator" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -229,13 +231,64 @@
   </si>
   <si>
     <t>Screen Size</t>
+  </si>
+  <si>
+    <t>Begin</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>Plane Size</t>
+  </si>
+  <si>
+    <t>Register Configuration</t>
+  </si>
+  <si>
+    <t>MMU_MAPn_SRC_LOWER</t>
+  </si>
+  <si>
+    <t>MMU_MAPn_SRC_UPPER</t>
+  </si>
+  <si>
+    <t>MMU_MAPn_TARGET</t>
+  </si>
+  <si>
+    <t>Total Graphics Size</t>
+  </si>
+  <si>
+    <t>Page Size</t>
+  </si>
+  <si>
+    <t>Plane Start</t>
+  </si>
+  <si>
+    <t>Stack Start</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +300,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,6 +343,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C2689D-9543-405F-B6B3-E28019047877}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -2267,4 +2341,224 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3FD334-D357-41C3-82E6-BD25F0D9B351}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="str">
+        <f>DEC2HEX(B4/I1)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>4000</v>
+      </c>
+      <c r="C3">
+        <v>6800</v>
+      </c>
+      <c r="D3">
+        <v>18000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="str">
+        <f>DEC2HEX(C4/I1)</f>
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3" t="str">
+        <f>"$" &amp; DEC2HEX(I3*1024)</f>
+        <v>$8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <f>HEX2DEC(B3)</f>
+        <v>16384</v>
+      </c>
+      <c r="C4" s="7">
+        <f>HEX2DEC(C3)</f>
+        <v>26624</v>
+      </c>
+      <c r="D4" s="7">
+        <f>HEX2DEC(D3)</f>
+        <v>98304</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="str">
+        <f>DEC2HEX(D4/I1)</f>
+        <v>C0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>64</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"$" &amp; DEC2HEX(I4*1024)</f>
+        <v>$10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="I5" s="5">
+        <f>SUM(I3:I4)</f>
+        <v>96</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"$" &amp; DEC2HEX(I5*1024)</f>
+        <v>$18000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7">
+        <f>320*256/8</f>
+        <v>10240</v>
+      </c>
+      <c r="J7" t="str">
+        <f>"$" &amp; DEC2HEX(I7)</f>
+        <v>$2800</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8">
+        <f>I7*4</f>
+        <v>40960</v>
+      </c>
+      <c r="J8" t="str">
+        <f>"$" &amp; DEC2HEX(I8)</f>
+        <v>$A000</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="9">
+        <v>391</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="9">
+        <f>DEC2HEX(F10+D4)*D11</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>32768</v>
+      </c>
+      <c r="J9" t="str">
+        <f>"$" &amp; DEC2HEX(I9)</f>
+        <v>$8000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="10">
+        <f>HEX2DEC(D9)</f>
+        <v>913</v>
+      </c>
+      <c r="F10" s="10">
+        <f>(D10-B4)*D11</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>256</v>
+      </c>
+      <c r="J10" t="str">
+        <f>"$" &amp; DEC2HEX(I10)</f>
+        <v>$100</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="10">
+        <f>IF(AND((D9&gt;=B3), (D9 &lt; C3)), 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Logging, ROM, and stack style
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Addresses" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Graphics" sheetId="3" r:id="rId4"/>
     <sheet name="Tiles" sheetId="4" r:id="rId5"/>
     <sheet name="Software MMU Calculator" sheetId="8" r:id="rId6"/>
+    <sheet name="Real Mode" sheetId="10" r:id="rId7"/>
+    <sheet name="Virtual Mode" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="118">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -282,13 +284,115 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>Accessable RAM</t>
+  </si>
+  <si>
+    <t>Number of Pages</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Virtual Addresses Common</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Registers</t>
+  </si>
+  <si>
+    <t>Rom</t>
+  </si>
+  <si>
+    <t>(Rom Copy)</t>
+  </si>
+  <si>
+    <t>Program Start</t>
+  </si>
+  <si>
+    <t>GPU Plane 1 (Default)</t>
+  </si>
+  <si>
+    <t>C00 Onwards</t>
+  </si>
+  <si>
+    <t>D800</t>
+  </si>
+  <si>
+    <t>E000</t>
+  </si>
+  <si>
+    <t>GPU Begin</t>
+  </si>
+  <si>
+    <t>GPU End</t>
+  </si>
+  <si>
+    <t>Real Mode is addressing when the virtual memory isn't on</t>
+  </si>
+  <si>
+    <t>In real mode, only the chip ram and ROM is accessible.</t>
+  </si>
+  <si>
+    <t>In virtual mode, all of the ram is accessible through page addressing. The ROM is not accessible (so has to be copied)</t>
+  </si>
+  <si>
+    <t>Chip Ram starts at 0 and ends at 8000</t>
+  </si>
+  <si>
+    <t>The GPU has direct access to the fast ram, but the CPU does not - it goes through the MMU.</t>
+  </si>
+  <si>
+    <t>Rom starts at 8000.</t>
+  </si>
+  <si>
+    <t>Anything after the ROM returns FEFE</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>(Repeats over and over)</t>
+  </si>
+  <si>
+    <t>Real Addressing</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Not accessible directly via CPU</t>
+  </si>
+  <si>
+    <t>PLANE_SIZE</t>
+  </si>
+  <si>
+    <t>Fast Page Finder</t>
+  </si>
+  <si>
+    <t>Fast Address</t>
+  </si>
+  <si>
+    <t>16-bit Page Finder</t>
+  </si>
+  <si>
+    <t>16-bit address</t>
+  </si>
+  <si>
+    <t>D400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +411,15 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,13 +445,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -357,6 +467,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,18 +1261,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2347,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3FD334-D357-41C3-82E6-BD25F0D9B351}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2392,7 +2513,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B3">
@@ -2423,15 +2544,15 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <f>HEX2DEC(B3)</f>
         <v>16384</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f>HEX2DEC(C3)</f>
         <v>26624</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <f>HEX2DEC(D3)</f>
         <v>98304</v>
       </c>
@@ -2455,7 +2576,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f>SUM(I3:I4)</f>
         <v>96</v>
       </c>
@@ -2504,16 +2625,16 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>391</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <f>DEC2HEX(F10+D4)*D11</f>
         <v>0</v>
       </c>
@@ -2529,11 +2650,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f>HEX2DEC(D9)</f>
         <v>913</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f>(D10-B4)*D11</f>
         <v>0</v>
       </c>
@@ -2549,13 +2670,577 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <f>IF(AND((D9&gt;=B3), (D9 &lt; C3)), 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7675F-5021-4351-84F4-26A676604FC9}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="str">
+        <f>DEC2HEX(J6*1024)</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>8000</v>
+      </c>
+      <c r="L7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I9" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="12">
+        <f>64*1024</f>
+        <v>65536</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="12" t="str">
+        <f>DEC2HEX(J10)</f>
+        <v>10000</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="8">
+        <f>320*256/8</f>
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G14" s="8" t="str">
+        <f>DEC2HEX(G13)</f>
+        <v>2800</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <f>J10-G13</f>
+        <v>55296</v>
+      </c>
+      <c r="L14" s="1" t="str">
+        <f>DEC2HEX(K14)</f>
+        <v>D800</v>
+      </c>
+      <c r="M14">
+        <f>K14+$G$13-1</f>
+        <v>65535</v>
+      </c>
+      <c r="N14" t="str">
+        <f>DEC2HEX(M14)</f>
+        <v>FFFF</v>
+      </c>
+      <c r="O14">
+        <f>16+(K14/1024)</f>
+        <v>70</v>
+      </c>
+      <c r="P14">
+        <f>16+INT(M14/1024)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>G13*4</f>
+        <v>40960</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13">
+        <f>K14-$G$13</f>
+        <v>45056</v>
+      </c>
+      <c r="L15" s="1" t="str">
+        <f t="shared" ref="L15:L17" si="0">DEC2HEX(K15)</f>
+        <v>B000</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M17" si="1">K15+$G$13-1</f>
+        <v>55295</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" ref="N15:N17" si="2">DEC2HEX(M15)</f>
+        <v>D7FF</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15:O17" si="3">16+K15/1024</f>
+        <v>60</v>
+      </c>
+      <c r="P15">
+        <f t="shared" ref="P15:P17" si="4">16+INT(M15/1024)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <v>2</v>
+      </c>
+      <c r="K16" s="13">
+        <f t="shared" ref="K16:K17" si="5">K15-$G$13</f>
+        <v>34816</v>
+      </c>
+      <c r="L16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>8800</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>45055</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="2"/>
+        <v>AFFF</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+      <c r="K17" s="13">
+        <f t="shared" si="5"/>
+        <v>24576</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>34815</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="2"/>
+        <v>87FF</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B202B4B7-4EBC-4356-AC3D-4D1D50087B26}">
+  <dimension ref="A1:R24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <f>SUM(A3:A4)*1024</f>
+        <v>81920</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1024</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5">
+        <f>320*256/8</f>
+        <v>10240</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5">
+        <f>F5*4</f>
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>F5/B5</f>
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6">
+        <f>B3-J5</f>
+        <v>40960</v>
+      </c>
+      <c r="K6" t="str">
+        <f>DEC2HEX(J6)</f>
+        <v>A000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>B3/B5</f>
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8">
+        <f>B3-J5</f>
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9">
+        <f>K8+J5</f>
+        <v>81920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" t="str">
+        <f>DEC2HEX(32*1024)</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12">
+        <v>512</v>
+      </c>
+      <c r="F12">
+        <f>INT(E12/B5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" ref="E16:E18" si="0">DEC2HEX(F16*$B$5)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17">
+        <v>400</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18">
+        <v>800</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N18" s="2" t="str">
+        <f>DEC2HEX(N19)</f>
+        <v>35</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f>DEC2HEX(R19)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f t="shared" ref="E19:E24" si="1">DEC2HEX(F19*$B$5)</f>
+        <v>C00</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+      <c r="M19" s="10">
+        <f>HEX2DEC(M18)</f>
+        <v>54272</v>
+      </c>
+      <c r="N19" s="10">
+        <f>M19/B5</f>
+        <v>53</v>
+      </c>
+      <c r="Q19" s="10">
+        <f>(A3*1024)+HEX2DEC(Q18)</f>
+        <v>71680</v>
+      </c>
+      <c r="R19" s="10">
+        <f>Q19/B5</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>8800</v>
+      </c>
+      <c r="F21">
+        <f>F20+10</f>
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>B000</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F24" si="2">F21+10</f>
+        <v>44</v>
+      </c>
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>D800</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Graphics System. Start on new Font.
</commit_message>
<xml_diff>
--- a/Documentation/MemoryLayout.xlsx
+++ b/Documentation/MemoryLayout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{7B50BA58-E4F6-4E5E-8A7B-EC7B56DD7C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Addresses" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="116">
   <si>
     <t>Chip Ram</t>
   </si>
@@ -322,9 +322,6 @@
     <t>C00 Onwards</t>
   </si>
   <si>
-    <t>D800</t>
-  </si>
-  <si>
     <t>E000</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
   </si>
   <si>
     <t>16-bit address</t>
-  </si>
-  <si>
-    <t>D400</t>
   </si>
 </sst>
 </file>
@@ -2700,25 +2694,25 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>36</v>
@@ -2736,7 +2730,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>91</v>
@@ -2748,25 +2742,25 @@
         <v>8000</v>
       </c>
       <c r="L7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" t="s">
         <v>107</v>
-      </c>
-      <c r="M7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="12">
         <f>64*1024</f>
@@ -2790,7 +2784,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="8">
         <f>320*256/8</f>
@@ -2950,7 +2944,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -3015,7 +3009,7 @@
         <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K8">
         <f>B3-J5</f>
@@ -3024,7 +3018,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9">
         <f>K8+J5</f>
@@ -3075,10 +3069,10 @@
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="5:18" x14ac:dyDescent="0.25">
@@ -3096,13 +3090,13 @@
         <v>400</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>89</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>89</v>
@@ -3126,11 +3120,11 @@
         <v>79</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="N18" s="2" t="str">
         <f>DEC2HEX(N19)</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5" t="s">
@@ -3141,7 +3135,7 @@
       </c>
       <c r="R18" s="2" t="str">
         <f>DEC2HEX(R19)</f>
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="5:18" x14ac:dyDescent="0.25">
@@ -3160,19 +3154,19 @@
       </c>
       <c r="M19" s="10">
         <f>HEX2DEC(M18)</f>
-        <v>54272</v>
+        <v>57344</v>
       </c>
       <c r="N19" s="10">
         <f>M19/B5</f>
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q19" s="10">
         <f>(A3*1024)+HEX2DEC(Q18)</f>
-        <v>71680</v>
+        <v>73728</v>
       </c>
       <c r="R19" s="10">
         <f>Q19/B5</f>
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="5:18" x14ac:dyDescent="0.25">
@@ -3187,7 +3181,7 @@
         <v>94</v>
       </c>
       <c r="H20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="5:18" x14ac:dyDescent="0.25">

</xml_diff>